<commit_message>
Normalization for CPF data
</commit_message>
<xml_diff>
--- a/Planilhas/Ferramentas/Ferramenta1-Github.xlsx
+++ b/Planilhas/Ferramentas/Ferramenta1-Github.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
   <si>
     <t xml:space="preserve">Assinante</t>
   </si>
@@ -46,9 +46,6 @@
     <t xml:space="preserve">398122745XX</t>
   </si>
   <si>
-    <t xml:space="preserve">254.63</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adriana Nogueira</t>
   </si>
   <si>
@@ -58,46 +55,43 @@
     <t xml:space="preserve">Afonso Barros</t>
   </si>
   <si>
-    <t xml:space="preserve">432.976.108-XX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">141.46</t>
+    <t xml:space="preserve">432976108XX</t>
   </si>
   <si>
     <t xml:space="preserve">Alan Esteves</t>
   </si>
   <si>
-    <t xml:space="preserve">215.630.874-XX</t>
+    <t xml:space="preserve">215630874XX</t>
   </si>
   <si>
     <t xml:space="preserve">Alberto da Luz</t>
   </si>
   <si>
-    <t xml:space="preserve">569.041.233-XX</t>
+    <t xml:space="preserve">569041233XX</t>
   </si>
   <si>
     <t xml:space="preserve">Alessandra Dias</t>
   </si>
   <si>
-    <t xml:space="preserve">088.714.596-XX</t>
+    <t xml:space="preserve">088714596XX</t>
   </si>
   <si>
     <t xml:space="preserve">Alexandre da Mata</t>
   </si>
   <si>
-    <t xml:space="preserve">321.458.907-XX</t>
+    <t xml:space="preserve">321458907XX</t>
   </si>
   <si>
     <t xml:space="preserve">Alice Farias</t>
   </si>
   <si>
-    <t xml:space="preserve">654.102.385-XX</t>
+    <t xml:space="preserve">654102385XX</t>
   </si>
   <si>
     <t xml:space="preserve">Aline da Rocha</t>
   </si>
   <si>
-    <t xml:space="preserve">987.546.721-XX</t>
+    <t xml:space="preserve">987546721XX</t>
   </si>
   <si>
     <t xml:space="preserve">Álvaro da Paz</t>
@@ -560,11 +554,11 @@
   </sheetPr>
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K45" activeCellId="0" sqref="K45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.38"/>
   </cols>
@@ -605,16 +599,16 @@
       <c r="E2" s="6" t="n">
         <v>141.46</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>8</v>
+      <c r="F2" s="7" t="n">
+        <v>254.63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>44693</v>
@@ -631,10 +625,10 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>45485</v>
@@ -645,16 +639,16 @@
       <c r="E4" s="6" t="n">
         <v>141.46</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>13</v>
+      <c r="F4" s="7" t="n">
+        <v>141.46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>45386</v>
@@ -671,10 +665,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>45163</v>
@@ -691,10 +685,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="8" t="n">
         <v>45645</v>
@@ -711,10 +705,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>45069</v>
@@ -731,10 +725,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>45554</v>
@@ -751,10 +745,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>45405</v>
@@ -771,10 +765,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>45670</v>
@@ -791,10 +785,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>45628</v>
@@ -811,10 +805,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>44693</v>
@@ -831,10 +825,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>44693</v>
@@ -851,10 +845,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>45677</v>
@@ -871,10 +865,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>44778</v>
@@ -891,10 +885,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>45684</v>
@@ -911,10 +905,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>45398</v>
@@ -931,10 +925,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" s="8" t="n">
         <v>45646</v>
@@ -951,10 +945,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="8" t="n">
         <v>45655</v>
@@ -971,10 +965,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>44693</v>
@@ -991,10 +985,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>44708</v>
@@ -1011,10 +1005,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>44770</v>
@@ -1031,10 +1025,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24" s="8" t="n">
         <v>44852</v>
@@ -1051,10 +1045,10 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>44704</v>
@@ -1071,10 +1065,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>45629</v>
@@ -1091,10 +1085,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="8" t="n">
         <v>45583</v>
@@ -1111,10 +1105,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>45510</v>
@@ -1131,10 +1125,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" s="8" t="n">
         <v>45618</v>
@@ -1151,10 +1145,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>45680</v>
@@ -1171,10 +1165,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="8" t="n">
         <v>44895</v>
@@ -1191,10 +1185,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>45343</v>
@@ -1211,10 +1205,10 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>45681</v>
@@ -1231,10 +1225,10 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>45378</v>
@@ -1251,10 +1245,10 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>45383</v>
@@ -1271,10 +1265,10 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>45552</v>
@@ -1291,10 +1285,10 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" s="8" t="n">
         <v>44894</v>
@@ -1311,10 +1305,10 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" s="8" t="n">
         <v>45644</v>
@@ -1331,10 +1325,10 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>45548</v>
@@ -1351,10 +1345,10 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>45057</v>
@@ -1371,10 +1365,10 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>44771</v>
@@ -1391,10 +1385,10 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C42" s="8" t="n">
         <v>45624</v>
@@ -1411,10 +1405,10 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>45163</v>
@@ -1431,10 +1425,10 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>45687</v>
@@ -1451,10 +1445,10 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C45" s="4" t="n">
         <v>45603</v>
@@ -1471,10 +1465,10 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>45526</v>
@@ -1491,10 +1485,10 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" s="4" t="n">
         <v>44704</v>
@@ -1511,10 +1505,10 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C48" s="4" t="n">
         <v>45517</v>
@@ -1531,10 +1525,10 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C49" s="8" t="n">
         <v>45624</v>
@@ -1551,10 +1545,10 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C50" s="4" t="n">
         <v>44693</v>
@@ -1571,10 +1565,10 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C51" s="4" t="n">
         <v>44780</v>
@@ -1591,10 +1585,10 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>45465</v>
@@ -1611,10 +1605,10 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>45553</v>
@@ -1625,16 +1619,16 @@
       <c r="E53" s="6" t="n">
         <v>141.46</v>
       </c>
-      <c r="F53" s="7" t="s">
-        <v>8</v>
+      <c r="F53" s="7" t="n">
+        <v>254.63</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>44693</v>
@@ -1651,10 +1645,10 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" s="8" t="n">
         <v>44894</v>
@@ -1671,10 +1665,10 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>45069</v>
@@ -1691,10 +1685,10 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>45021</v>
@@ -1711,10 +1705,10 @@
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>45510</v>
@@ -1731,10 +1725,10 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C59" s="4" t="n">
         <v>45672</v>
@@ -1751,10 +1745,10 @@
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C60" s="4" t="n">
         <v>44720</v>
@@ -1771,10 +1765,10 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C61" s="4" t="n">
         <v>45327</v>
@@ -1791,10 +1785,10 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>45426</v>
@@ -1811,10 +1805,10 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C63" s="4" t="n">
         <v>44713</v>

</xml_diff>